<commit_message>
solved formatting errors for now, reading excel cells has error that needs solution. code is non-functional
</commit_message>
<xml_diff>
--- a/src/main/resources/Cut Sheet Express excel.xlsx
+++ b/src/main/resources/Cut Sheet Express excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Computer Programming Projects\GitHub\Meta-Cut-Sheet\Meta-Cut-Sheet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096F25DF-3816-47C7-9C93-E3A923CAD756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EFA050-1503-49A5-A61E-C539FC2D26DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{883FB1BF-892E-4411-9927-2E16DAD06FFC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Approved By:</t>
   </si>
@@ -95,33 +95,6 @@
   </si>
   <si>
     <t>Dimmable:</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>f</t>
   </si>
 </sst>
 </file>
@@ -483,7 +456,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -591,146 +564,103 @@
       <c r="I2">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <v>13</v>
+      </c>
+      <c r="N2">
+        <v>14</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
+      <c r="P2">
+        <v>16</v>
+      </c>
+      <c r="Q2">
+        <v>17</v>
+      </c>
+      <c r="R2">
+        <v>18</v>
+      </c>
+      <c r="S2">
+        <v>19</v>
+      </c>
+      <c r="T2">
         <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="G3">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="H3">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="I3">
-        <v>9</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="J3">
+        <v>30</v>
+      </c>
+      <c r="K3">
+        <v>31</v>
+      </c>
+      <c r="L3">
+        <v>32</v>
+      </c>
+      <c r="M3">
+        <v>33</v>
+      </c>
+      <c r="N3">
+        <v>34</v>
+      </c>
+      <c r="O3">
+        <v>35</v>
+      </c>
+      <c r="P3">
+        <v>36</v>
+      </c>
+      <c r="Q3">
+        <v>37</v>
+      </c>
+      <c r="R3">
+        <v>38</v>
+      </c>
+      <c r="S3">
+        <v>39</v>
+      </c>
+      <c r="T3">
+        <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>7</v>
-      </c>
-      <c r="H4">
-        <v>8</v>
-      </c>
-      <c r="I4">
-        <v>9</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R4" t="s">
-        <v>28</v>
-      </c>
-    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
     </row>

</xml_diff>

<commit_message>
reading excel cells still has error that needs solution. code is non-functional
</commit_message>
<xml_diff>
--- a/src/main/resources/Cut Sheet Express excel.xlsx
+++ b/src/main/resources/Cut Sheet Express excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Computer Programming Projects\GitHub\Meta-Cut-Sheet\Meta-Cut-Sheet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EFA050-1503-49A5-A61E-C539FC2D26DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCDC61F-A0D3-4F66-9B99-3355976E742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{883FB1BF-892E-4411-9927-2E16DAD06FFC}"/>
   </bookViews>
@@ -453,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6172A9D-621C-4832-85CA-1476DE915E32}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A4" sqref="A4:T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,76 +600,67 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T3">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
successful in reading excel data and filling hard coded data into form, need to combine both methods
</commit_message>
<xml_diff>
--- a/src/main/resources/Cut Sheet Express excel.xlsx
+++ b/src/main/resources/Cut Sheet Express excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Computer Programming Projects\GitHub\Meta-Cut-Sheet\Meta-Cut-Sheet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCDC61F-A0D3-4F66-9B99-3355976E742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEC70CB-9904-436D-BB79-1EDA20D050B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{883FB1BF-892E-4411-9927-2E16DAD06FFC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Approved By:</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Dimmable:</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -136,9 +139,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6172A9D-621C-4832-85CA-1476DE915E32}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:T20"/>
+      <selection activeCell="A6" sqref="A6:XFD141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,7 +488,7 @@
       <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D1" t="s">
@@ -600,67 +607,190 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3">
         <v>22</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>23</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>24</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>25</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>26</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>27</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>28</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>29</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>30</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>31</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>32</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>33</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>34</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>35</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>36</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>37</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>38</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>39</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>40</v>
       </c>
-      <c r="T3">
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>41</v>
       </c>
+      <c r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>43</v>
+      </c>
+      <c r="D4">
+        <v>44</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>46</v>
+      </c>
+      <c r="G4">
+        <v>47</v>
+      </c>
+      <c r="H4">
+        <v>48</v>
+      </c>
+      <c r="I4">
+        <v>49</v>
+      </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>51</v>
+      </c>
+      <c r="L4">
+        <v>52</v>
+      </c>
+      <c r="M4">
+        <v>53</v>
+      </c>
+      <c r="N4">
+        <v>54</v>
+      </c>
+      <c r="O4">
+        <v>55</v>
+      </c>
+      <c r="P4">
+        <v>56</v>
+      </c>
+      <c r="Q4">
+        <v>57</v>
+      </c>
+      <c r="R4">
+        <v>58</v>
+      </c>
+      <c r="S4">
+        <v>59</v>
+      </c>
+      <c r="T4">
+        <v>60</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
solved error, needs better logic for null cells. restructure planning still in progress
</commit_message>
<xml_diff>
--- a/src/main/resources/Cut Sheet Express excel.xlsx
+++ b/src/main/resources/Cut Sheet Express excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Computer Programming Projects\GitHub\Meta-Cut-Sheet\Meta-Cut-Sheet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC97679-E492-4140-9985-6BF2A8EC812E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BC25EE-6D16-4E00-8E63-AF85C7326094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{883FB1BF-892E-4411-9927-2E16DAD06FFC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
   <si>
     <t>Approved By:</t>
   </si>
@@ -135,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +145,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,19 +167,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -184,6 +203,36 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{852DA304-7032-4618-B511-217449900421}" name="Table1" displayName="Table1" ref="A1:U100" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:U100" xr:uid="{852DA304-7032-4618-B511-217449900421}"/>
+  <tableColumns count="21">
+    <tableColumn id="1" xr3:uid="{9D19FFFA-B775-4489-9390-36C76AFEF98A}" name="Fixture/Device:"/>
+    <tableColumn id="2" xr3:uid="{78D8E6E6-DCF9-483A-A46E-7F3E881850B1}" name="PDF/Images"/>
+    <tableColumn id="3" xr3:uid="{70494E44-73AA-429E-81D7-ECCB179BA18C}" name="Taget PDF/Image Location  "/>
+    <tableColumn id="4" xr3:uid="{D5B47E2C-5E1B-4214-8B24-66B39CA67450}" name="Save Location"/>
+    <tableColumn id="5" xr3:uid="{A257C42C-962D-4925-963A-7F6289564777}" name="Type:"/>
+    <tableColumn id="6" xr3:uid="{0B48EE76-4F4F-48DB-BB69-C1E64813295A}" name="Manufacturer:"/>
+    <tableColumn id="7" xr3:uid="{6D636A0E-C231-41CF-A0CB-0F7B06CA4780}" name="Model #:"/>
+    <tableColumn id="8" xr3:uid="{34C47792-DC99-437C-8F61-D6503EB0C8AE}" name="Part #:"/>
+    <tableColumn id="9" xr3:uid="{7F1830D6-F0E5-4D32-BA02-051125BFC4FC}" name="Description:"/>
+    <tableColumn id="10" xr3:uid="{787AF3E6-8691-4D1D-9065-070811E9B0E1}" name="Wattage:"/>
+    <tableColumn id="11" xr3:uid="{CA703666-7AAF-435A-9C47-8055537FBDAC}" name="Voltage:"/>
+    <tableColumn id="12" xr3:uid="{77FA695F-7DDD-4E40-8696-161C78AE79B9}" name="Control:"/>
+    <tableColumn id="13" xr3:uid="{59F793B5-CA15-461F-9521-BC13205353FE}" name="Dimmable:"/>
+    <tableColumn id="14" xr3:uid="{13FEBC5F-6D69-4567-A39E-98D9AFEEE1CE}" name="Date:" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{2C2FE7BD-898F-45BD-8F3D-C82D6A3A90C8}" name="Revision:"/>
+    <tableColumn id="16" xr3:uid="{8D421A21-05EF-45DE-BCE5-5D8A1143EB0B}" name="Approved By:"/>
+    <tableColumn id="17" xr3:uid="{FF2DABBD-90CC-45A0-BD5C-FF6513B88874}" name="LD:"/>
+    <tableColumn id="18" xr3:uid="{049D9B48-9389-460F-A28F-C193ACD2F2D5}" name="Design Firm:"/>
+    <tableColumn id="19" xr3:uid="{23E47C72-F59D-4986-8CB8-1513EEA69DA1}" name="Project Name:"/>
+    <tableColumn id="20" xr3:uid="{146E7070-6432-4E82-9543-EC7110D9093F}" name="Project Location:"/>
+    <tableColumn id="21" xr3:uid="{405B5825-E346-4B9A-97E3-69FAF4B03744}" name="Notes:"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,91 +534,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6172A9D-621C-4832-85CA-1476DE915E32}">
   <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="J3" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" customWidth="1"/>
     <col min="4" max="4" width="27.1796875" customWidth="1"/>
     <col min="5" max="5" width="10.90625" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="10" max="10" width="10.36328125" customWidth="1"/>
+    <col min="11" max="12" width="9.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.90625" customWidth="1"/>
     <col min="14" max="14" width="21.1796875" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.26953125" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="18" max="18" width="13.08984375" customWidth="1"/>
+    <col min="19" max="19" width="14.453125" customWidth="1"/>
+    <col min="20" max="20" width="16.54296875" customWidth="1"/>
     <col min="21" max="21" width="20.6328125" customWidth="1"/>
     <col min="22" max="22" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -613,9 +667,9 @@
       <c r="M2">
         <v>9</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <f ca="1">NOW()</f>
-        <v>45610.948402430557</v>
+        <v>45614.930392824077</v>
       </c>
       <c r="O2">
         <v>11</v>
@@ -679,9 +733,9 @@
       <c r="M3">
         <v>29</v>
       </c>
-      <c r="N3" s="4">
-        <f t="shared" ref="N3:N66" ca="1" si="0">NOW()</f>
-        <v>45610.948402430557</v>
+      <c r="N3" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45614</v>
       </c>
       <c r="O3">
         <v>31</v>
@@ -745,9 +799,9 @@
       <c r="M4">
         <v>49</v>
       </c>
-      <c r="N4" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>45610.948402430557</v>
+      <c r="N4" s="3">
+        <f t="shared" ref="N4:N14" ca="1" si="0">TODAY()</f>
+        <v>45614</v>
       </c>
       <c r="O4">
         <v>51</v>
@@ -811,9 +865,9 @@
       <c r="M5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45610.948402430557</v>
+        <v>45614</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>18</v>
@@ -877,9 +931,9 @@
       <c r="M6">
         <v>9</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45610.948402430557</v>
+        <v>45614</v>
       </c>
       <c r="O6">
         <v>11</v>
@@ -943,9 +997,9 @@
       <c r="M7">
         <v>13</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45610.948402430557</v>
+        <v>45614</v>
       </c>
       <c r="O7">
         <v>15</v>
@@ -1009,9 +1063,9 @@
       <c r="M8">
         <v>18</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45610.948402430557</v>
+        <v>45614</v>
       </c>
       <c r="O8">
         <v>20</v>
@@ -1075,9 +1129,9 @@
       <c r="M9">
         <v>28</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45610.948402430557</v>
+        <v>45614</v>
       </c>
       <c r="O9">
         <v>30</v>
@@ -1141,9 +1195,9 @@
       <c r="M10">
         <v>38</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45610.948402430557</v>
+        <v>45614</v>
       </c>
       <c r="O10">
         <v>40</v>
@@ -1207,9 +1261,9 @@
       <c r="M11">
         <v>48</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45610.948402430557</v>
+        <v>45614</v>
       </c>
       <c r="O11">
         <v>50</v>
@@ -1273,9 +1327,9 @@
       <c r="M12">
         <v>58</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45610.948402430557</v>
+        <v>45614</v>
       </c>
       <c r="O12">
         <v>60</v>
@@ -1339,9 +1393,9 @@
       <c r="M13">
         <v>68</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45610.948402430557</v>
+        <v>45614</v>
       </c>
       <c r="O13">
         <v>70</v>
@@ -1366,269 +1420,287 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="N14" s="4"/>
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14">
+        <v>60</v>
+      </c>
+      <c r="G14">
+        <v>62</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45614</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="N15" s="4"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="N16" s="4"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N17" s="4"/>
+      <c r="N17" s="3"/>
     </row>
     <row r="18" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N18" s="4"/>
+      <c r="N18" s="3"/>
     </row>
     <row r="19" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N19" s="4"/>
+      <c r="N19" s="3"/>
     </row>
     <row r="20" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N20" s="4"/>
+      <c r="N20" s="3"/>
     </row>
     <row r="21" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N21" s="4"/>
+      <c r="N21" s="3"/>
     </row>
     <row r="22" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N22" s="4"/>
+      <c r="N22" s="3"/>
     </row>
     <row r="23" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N23" s="4"/>
+      <c r="N23" s="3"/>
     </row>
     <row r="24" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N24" s="4"/>
+      <c r="N24" s="3"/>
     </row>
     <row r="25" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N25" s="4"/>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N26" s="4"/>
+      <c r="N26" s="3"/>
     </row>
     <row r="27" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N27" s="4"/>
+      <c r="N27" s="3"/>
     </row>
     <row r="28" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N28" s="4"/>
+      <c r="N28" s="3"/>
     </row>
     <row r="29" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N29" s="4"/>
+      <c r="N29" s="3"/>
     </row>
     <row r="30" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N30" s="4"/>
+      <c r="N30" s="3"/>
     </row>
     <row r="31" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N31" s="4"/>
+      <c r="N31" s="3"/>
     </row>
     <row r="32" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N32" s="4"/>
+      <c r="N32" s="3"/>
     </row>
     <row r="33" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N33" s="4"/>
+      <c r="N33" s="3"/>
     </row>
     <row r="34" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N34" s="4"/>
+      <c r="N34" s="3"/>
     </row>
     <row r="35" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N35" s="4"/>
+      <c r="N35" s="3"/>
     </row>
     <row r="36" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N36" s="4"/>
+      <c r="N36" s="3"/>
     </row>
     <row r="37" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N37" s="4"/>
+      <c r="N37" s="3"/>
     </row>
     <row r="38" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N38" s="4"/>
+      <c r="N38" s="3"/>
     </row>
     <row r="39" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N39" s="4"/>
+      <c r="N39" s="3"/>
     </row>
     <row r="40" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N40" s="4"/>
+      <c r="N40" s="3"/>
     </row>
     <row r="41" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N41" s="4"/>
+      <c r="N41" s="3"/>
     </row>
     <row r="42" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N42" s="4"/>
+      <c r="N42" s="3"/>
     </row>
     <row r="43" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N43" s="4"/>
+      <c r="N43" s="3"/>
     </row>
     <row r="44" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N44" s="4"/>
+      <c r="N44" s="3"/>
     </row>
     <row r="45" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N45" s="4"/>
+      <c r="N45" s="3"/>
     </row>
     <row r="46" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N46" s="4"/>
+      <c r="N46" s="3"/>
     </row>
     <row r="47" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N47" s="4"/>
+      <c r="N47" s="3"/>
     </row>
     <row r="48" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N48" s="4"/>
+      <c r="N48" s="3"/>
     </row>
     <row r="49" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N49" s="4"/>
+      <c r="N49" s="3"/>
     </row>
     <row r="50" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N50" s="4"/>
+      <c r="N50" s="3"/>
     </row>
     <row r="51" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N51" s="4"/>
+      <c r="N51" s="3"/>
     </row>
     <row r="52" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N52" s="4"/>
+      <c r="N52" s="3"/>
     </row>
     <row r="53" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N53" s="4"/>
+      <c r="N53" s="3"/>
     </row>
     <row r="54" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N54" s="4"/>
+      <c r="N54" s="3"/>
     </row>
     <row r="55" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N55" s="4"/>
+      <c r="N55" s="3"/>
     </row>
     <row r="56" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N56" s="4"/>
+      <c r="N56" s="3"/>
     </row>
     <row r="57" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N57" s="4"/>
+      <c r="N57" s="3"/>
     </row>
     <row r="58" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N58" s="4"/>
+      <c r="N58" s="3"/>
     </row>
     <row r="59" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N59" s="4"/>
+      <c r="N59" s="3"/>
     </row>
     <row r="60" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N60" s="4"/>
+      <c r="N60" s="3"/>
     </row>
     <row r="61" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N61" s="4"/>
+      <c r="N61" s="3"/>
     </row>
     <row r="62" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N62" s="4"/>
+      <c r="N62" s="3"/>
     </row>
     <row r="63" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N63" s="4"/>
+      <c r="N63" s="3"/>
     </row>
     <row r="64" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N64" s="4"/>
+      <c r="N64" s="3"/>
     </row>
     <row r="65" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N65" s="4"/>
+      <c r="N65" s="3"/>
     </row>
     <row r="66" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N66" s="4"/>
+      <c r="N66" s="3"/>
     </row>
     <row r="67" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N67" s="4"/>
+      <c r="N67" s="3"/>
     </row>
     <row r="68" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N68" s="4"/>
+      <c r="N68" s="3"/>
     </row>
     <row r="69" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N69" s="4"/>
+      <c r="N69" s="3"/>
     </row>
     <row r="70" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N70" s="4"/>
+      <c r="N70" s="3"/>
     </row>
     <row r="71" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N71" s="4"/>
+      <c r="N71" s="3"/>
     </row>
     <row r="72" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N72" s="4"/>
+      <c r="N72" s="3"/>
     </row>
     <row r="73" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N73" s="4"/>
+      <c r="N73" s="3"/>
     </row>
     <row r="74" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N74" s="4"/>
+      <c r="N74" s="3"/>
     </row>
     <row r="75" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N75" s="4"/>
+      <c r="N75" s="3"/>
     </row>
     <row r="76" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N76" s="4"/>
+      <c r="N76" s="3"/>
     </row>
     <row r="77" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N77" s="4"/>
+      <c r="N77" s="3"/>
     </row>
     <row r="78" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N78" s="4"/>
+      <c r="N78" s="3"/>
     </row>
     <row r="79" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N79" s="4"/>
+      <c r="N79" s="3"/>
     </row>
     <row r="80" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N80" s="4"/>
+      <c r="N80" s="3"/>
     </row>
     <row r="81" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N81" s="4"/>
+      <c r="N81" s="3"/>
     </row>
     <row r="82" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N82" s="4"/>
+      <c r="N82" s="3"/>
     </row>
     <row r="83" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N83" s="4"/>
+      <c r="N83" s="3"/>
     </row>
     <row r="84" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N84" s="4"/>
+      <c r="N84" s="3"/>
     </row>
     <row r="85" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N85" s="4"/>
+      <c r="N85" s="3"/>
     </row>
     <row r="86" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N86" s="4"/>
+      <c r="N86" s="3"/>
     </row>
     <row r="87" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N87" s="4"/>
+      <c r="N87" s="3"/>
     </row>
     <row r="88" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N88" s="4"/>
+      <c r="N88" s="3"/>
     </row>
     <row r="89" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N89" s="4"/>
+      <c r="N89" s="3"/>
     </row>
     <row r="90" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N90" s="4"/>
+      <c r="N90" s="3"/>
     </row>
     <row r="91" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N91" s="4"/>
+      <c r="N91" s="3"/>
     </row>
     <row r="92" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N92" s="4"/>
+      <c r="N92" s="3"/>
     </row>
     <row r="93" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N93" s="4"/>
+      <c r="N93" s="3"/>
     </row>
     <row r="94" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N94" s="4"/>
+      <c r="N94" s="3"/>
     </row>
     <row r="95" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N95" s="4"/>
+      <c r="N95" s="3"/>
     </row>
     <row r="96" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N96" s="4"/>
+      <c r="N96" s="3"/>
     </row>
     <row r="97" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N97" s="4"/>
+      <c r="N97" s="3"/>
     </row>
     <row r="98" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N98" s="4"/>
+      <c r="N98" s="3"/>
     </row>
     <row r="99" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N99" s="4"/>
+      <c r="N99" s="3"/>
     </row>
     <row r="100" spans="14:14" x14ac:dyDescent="0.35">
-      <c r="N100" s="4"/>
+      <c r="N100" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
Successfully implemented map lists for data storage. working on data recall and manipulation to fill forms.
</commit_message>
<xml_diff>
--- a/src/main/resources/Cut Sheet Express excel.xlsx
+++ b/src/main/resources/Cut Sheet Express excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Computer Programming Projects\GitHub\Meta-Cut-Sheet\Meta-Cut-Sheet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78D2C17-7F1E-4869-826C-9FD271423BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50A3610-D649-4024-9BFC-B0572B248824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23232" yWindow="2040" windowWidth="14400" windowHeight="7356" xr2:uid="{883FB1BF-892E-4411-9927-2E16DAD06FFC}"/>
+    <workbookView xWindow="22932" yWindow="1860" windowWidth="16536" windowHeight="8832" xr2:uid="{883FB1BF-892E-4411-9927-2E16DAD06FFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="41">
   <si>
     <t>Approved By:</t>
   </si>
@@ -95,9 +95,6 @@
     <t>a</t>
   </si>
   <si>
-    <t>Save Location</t>
-  </si>
-  <si>
     <t>C:\Users\James\Desktop\temp</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>Images</t>
   </si>
   <si>
-    <t xml:space="preserve">Target PDF/Image Location  </t>
-  </si>
-  <si>
     <t>C:\Users\James\Desktop\001</t>
   </si>
   <si>
@@ -156,13 +150,22 @@
   </si>
   <si>
     <t>C:\Users\James\Desktop\013</t>
+  </si>
+  <si>
+    <t>PDF/Images:</t>
+  </si>
+  <si>
+    <t>Save Location:</t>
+  </si>
+  <si>
+    <t>Target PDF/Image Location:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +175,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -209,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -226,6 +237,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -320,8 +332,8 @@
   <autoFilter ref="B1:U100" xr:uid="{852DA304-7032-4618-B511-217449900421}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{9D19FFFA-B775-4489-9390-36C76AFEF98A}" name="Fixture/Device:" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{78D8E6E6-DCF9-483A-A46E-7F3E881850B1}" name="PDF/Images" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{D5B47E2C-5E1B-4214-8B24-66B39CA67450}" name="Save Location" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{78D8E6E6-DCF9-483A-A46E-7F3E881850B1}" name="PDF/Images:" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{D5B47E2C-5E1B-4214-8B24-66B39CA67450}" name="Save Location:" dataDxfId="17"/>
     <tableColumn id="5" xr3:uid="{A257C42C-962D-4925-963A-7F6289564777}" name="Type:" dataDxfId="16"/>
     <tableColumn id="6" xr3:uid="{0B48EE76-4F4F-48DB-BB69-C1E64813295A}" name="Manufacturer:" dataDxfId="15"/>
     <tableColumn id="7" xr3:uid="{6D636A0E-C231-41CF-A0CB-0F7B06CA4780}" name="Model #:" dataDxfId="14"/>
@@ -643,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6172A9D-621C-4832-85CA-1476DE915E32}">
   <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,17 +684,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>26</v>
+      <c r="A1" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>6</v>
@@ -738,16 +750,16 @@
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -778,7 +790,7 @@
       </c>
       <c r="N2" s="5">
         <f ca="1">NOW()</f>
-        <v>45615.934743287035</v>
+        <v>45628.922569907409</v>
       </c>
       <c r="O2" s="5">
         <v>11</v>
@@ -804,16 +816,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="5">
         <v>21</v>
@@ -844,7 +856,7 @@
       </c>
       <c r="N3" s="5">
         <f ca="1">TODAY()</f>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O3" s="5">
         <v>31</v>
@@ -870,16 +882,16 @@
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="5">
         <v>41</v>
@@ -910,7 +922,7 @@
       </c>
       <c r="N4" s="5">
         <f t="shared" ref="N4:N14" ca="1" si="0">TODAY()</f>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O4" s="5">
         <v>51</v>
@@ -936,16 +948,16 @@
     </row>
     <row r="5" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>18</v>
@@ -976,7 +988,7 @@
       </c>
       <c r="N5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>18</v>
@@ -1002,16 +1014,16 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -1042,7 +1054,7 @@
       </c>
       <c r="N6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O6" s="5">
         <v>11</v>
@@ -1068,16 +1080,16 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="5">
         <v>5</v>
@@ -1108,7 +1120,7 @@
       </c>
       <c r="N7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O7" s="5">
         <v>15</v>
@@ -1134,16 +1146,16 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="5">
         <v>10</v>
@@ -1174,7 +1186,7 @@
       </c>
       <c r="N8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O8" s="5">
         <v>20</v>
@@ -1200,16 +1212,16 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="5">
         <v>20</v>
@@ -1240,7 +1252,7 @@
       </c>
       <c r="N9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O9" s="5">
         <v>30</v>
@@ -1266,16 +1278,16 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="5">
         <v>30</v>
@@ -1306,7 +1318,7 @@
       </c>
       <c r="N10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O10" s="5">
         <v>40</v>
@@ -1332,16 +1344,16 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="5">
         <v>40</v>
@@ -1372,7 +1384,7 @@
       </c>
       <c r="N11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O11" s="5">
         <v>50</v>
@@ -1398,16 +1410,16 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="5">
         <v>50</v>
@@ -1438,7 +1450,7 @@
       </c>
       <c r="N12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O12" s="5">
         <v>60</v>
@@ -1464,16 +1476,16 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5">
         <v>60</v>
@@ -1504,7 +1516,7 @@
       </c>
       <c r="N13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O13" s="5">
         <v>70</v>
@@ -1530,10 +1542,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1552,7 +1564,7 @@
       <c r="M14" s="5"/>
       <c r="N14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45615</v>
+        <v>45628</v>
       </c>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
@@ -3587,23 +3599,23 @@
         <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>